<commit_message>
Fixed sprint dates on sprint 4 plan
</commit_message>
<xml_diff>
--- a/sprint_backlog/sprint4/plan.xlsx
+++ b/sprint_backlog/sprint4/plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\ajg\Documents (D)\Repositories\CSCC01\Team5\sprint_backlog\sprint4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D485A6C-C355-4F64-ADD3-92A974F19B94}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C451946-F601-4F53-BAF2-E2A52829D39C}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="36">
   <si>
     <r>
       <rPr>
@@ -137,9 +137,6 @@
     <t>X</t>
   </si>
   <si>
-    <t>Sprint 3 Plan (Oct 30 - Nov 3)</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -162,6 +159,12 @@
   </si>
   <si>
     <t>T7, T8, T9</t>
+  </si>
+  <si>
+    <t>Saad thinks that he will be able to complete T15 in 3 story points instead of 5 as originally estimated</t>
+  </si>
+  <si>
+    <t>Sprint 4 Plan (Nov 6 - Nov 10)</t>
   </si>
 </sst>
 </file>
@@ -301,7 +304,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -709,7 +712,7 @@
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="A2" sqref="A2:J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -725,7 +728,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -806,7 +809,9 @@
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
+      <c r="J4" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
@@ -816,25 +821,25 @@
         <v>16</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D5" s="3">
         <v>5</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>25</v>
@@ -871,10 +876,10 @@
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
       <c r="B7" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D7" s="3">
         <v>5</v>
@@ -895,7 +900,7 @@
         <v>19</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>21</v>
@@ -907,10 +912,10 @@
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J8" s="3" t="s">
         <v>25</v>
@@ -924,27 +929,29 @@
         <v>23</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D9" s="3">
         <v>3</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
+      <c r="J9" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B12" s="14"/>
       <c r="C12" s="14"/>
@@ -957,7 +964,9 @@
       <c r="J12" s="14"/>
     </row>
     <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
+      <c r="A13" s="7" t="s">
+        <v>34</v>
+      </c>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>

</xml_diff>